<commit_message>
Updated A_mueller affiliations, Updated Holly page (to former members)
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Ashley_Mueller/Author_form_380 (Copy).xlsx
+++ b/website_content_creation/authors/Ashley_Mueller/Author_form_380 (Copy).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Summer Student Technician</t>
+  </si>
+  <si>
+    <t>Great Lakes Forestry Centre, Natural Resources Canada</t>
+  </si>
+  <si>
+    <t>https://www.nrcan.gc.ca/science-data/research-centres-labs/forestry-research-centres/great-lakes-forestry-centre/13459</t>
   </si>
 </sst>
 </file>
@@ -741,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -920,8 +926,12 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>

</xml_diff>

<commit_message>
updated all e-mails, publications from google scholar
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Ashley_Mueller/Author_form_380 (Copy).xlsx
+++ b/website_content_creation/authors/Ashley_Mueller/Author_form_380 (Copy).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\Documents\WET lab\WETlab_website\website_content_creation\authors\Ashley_Mueller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\RProjects\GLFC-WET.github.io\website_content_creation\authors\Ashley_Mueller\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -98,9 +98,6 @@
     <t>Ashley Mueller</t>
   </si>
   <si>
-    <t>ashley.mueller@canada.ca</t>
-  </si>
-  <si>
     <t>linkedin.com/in/ashley-mueller-2106891b4</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>Past WETlab Members</t>
+  </si>
+  <si>
+    <t>ashley.mueller@NRCan-RNCan.gc.ca</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
@@ -529,6 +528,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -748,7 +748,7 @@
   <dimension ref="A1:C1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -771,7 +771,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -779,70 +779,70 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="23"/>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+    </row>
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="25"/>
-    </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="26" t="s">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="25"/>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="23"/>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>22</v>
@@ -854,11 +854,11 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
@@ -873,10 +873,10 @@
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C16" s="2">
         <v>2023</v>
@@ -904,10 +904,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="33"/>
+      <c r="B22" s="32"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
@@ -919,18 +919,18 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -961,27 +961,27 @@
     </row>
     <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>